<commit_message>
updates sample for Tanium
</commit_message>
<xml_diff>
--- a/Tanium_data_sample.xlsx
+++ b/Tanium_data_sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/novo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/novo/Dev/t4sg/Rationalization2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFFF02DE-77BB-554E-AF54-445BA050C6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1FBA7C-114D-A84F-BBF1-B01F81A03E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A5011033-20C1-A54F-876B-D3140F936B03}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A5011033-20C1-A54F-876B-D3140F936B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -779,46 +779,67 @@
   <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>56</v>
-      </c>
-      <c r="E1" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>20</v>
       </c>
       <c r="E2" s="1">
         <v>44575.086921296293</v>
@@ -829,95 +850,95 @@
       <c r="G2" t="s">
         <v>60</v>
       </c>
-      <c r="K2" t="s">
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" t="s">
         <v>54</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O3" t="s">
         <v>25</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E4" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" t="s">
         <v>3</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P4" t="s">
         <v>1</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E5" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F5" t="s">
         <v>118</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L5" t="s">
         <v>26</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M5" t="s">
         <v>25</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" t="s">
-        <v>125</v>
-      </c>
-      <c r="K5" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s">
-        <v>25</v>
-      </c>
-      <c r="S5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>108</v>
       </c>
@@ -925,31 +946,31 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
+        <v>125</v>
       </c>
       <c r="K6" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="L6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>3</v>
-      </c>
-      <c r="P6" t="s">
-        <v>2</v>
-      </c>
-      <c r="R6" t="s">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
+        <v>25</v>
       </c>
       <c r="S6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>108</v>
       </c>
@@ -957,68 +978,65 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>60</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I8" t="s">
         <v>59</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K8" t="s">
         <v>54</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L8" t="s">
         <v>31</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O8" t="s">
         <v>26</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P8" t="s">
         <v>25</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>56</v>
-      </c>
-      <c r="E8" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" t="s">
-        <v>121</v>
-      </c>
-      <c r="N8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" t="s">
-        <v>25</v>
-      </c>
-      <c r="S8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>108</v>
       </c>
       <c r="E9" s="1">
         <v>44575.086921296293</v>
@@ -1027,28 +1045,31 @@
         <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" t="s">
+        <v>121</v>
+      </c>
+      <c r="N9" t="s">
         <v>5</v>
       </c>
-      <c r="M9" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" t="s">
-        <v>3</v>
+      <c r="O9" t="s">
+        <v>44</v>
       </c>
       <c r="P9" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="R9" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="S9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>108</v>
       </c>
@@ -1056,37 +1077,31 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
       <c r="L10" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="M10" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="N10" t="s">
-        <v>114</v>
-      </c>
-      <c r="O10" t="s">
-        <v>113</v>
+        <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="R10" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="S10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>108</v>
       </c>
@@ -1094,95 +1109,101 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" t="s">
+        <v>117</v>
+      </c>
+      <c r="L11" t="s">
+        <v>116</v>
+      </c>
+      <c r="M11" t="s">
+        <v>115</v>
+      </c>
+      <c r="N11" t="s">
+        <v>114</v>
+      </c>
+      <c r="O11" t="s">
+        <v>113</v>
+      </c>
+      <c r="P11" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>111</v>
+      </c>
+      <c r="R11" t="s">
+        <v>110</v>
+      </c>
+      <c r="S11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F12" t="s">
         <v>29</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>60</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>59</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>54</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>31</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O12" t="s">
         <v>26</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P12" t="s">
         <v>25</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F12" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F13" t="s">
         <v>40</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>39</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>38</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J13" s="1">
         <v>44573.75</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K13" t="s">
         <v>106</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L13" t="s">
         <v>105</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="1">
-        <v>44574.75</v>
-      </c>
-      <c r="K13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" t="s">
-        <v>73</v>
-      </c>
-      <c r="S13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>41</v>
       </c>
@@ -1205,16 +1226,16 @@
         <v>44574.75</v>
       </c>
       <c r="K14" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="L14" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="S14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>41</v>
       </c>
@@ -1237,16 +1258,16 @@
         <v>44574.75</v>
       </c>
       <c r="K15" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="L15" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="S15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>41</v>
       </c>
@@ -1269,10 +1290,10 @@
         <v>44574.75</v>
       </c>
       <c r="K16" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="L16" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="S16" t="s">
         <v>102</v>
@@ -1307,7 +1328,7 @@
         <v>43</v>
       </c>
       <c r="S17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.2">
@@ -1333,16 +1354,13 @@
         <v>44574.75</v>
       </c>
       <c r="K18" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="L18" t="s">
-        <v>31</v>
-      </c>
-      <c r="M18" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="S18" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.2">
@@ -1368,13 +1386,16 @@
         <v>44574.75</v>
       </c>
       <c r="K19" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="L19" t="s">
-        <v>73</v>
+        <v>31</v>
+      </c>
+      <c r="M19" t="s">
+        <v>32</v>
       </c>
       <c r="S19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.2">
@@ -1400,10 +1421,10 @@
         <v>44574.75</v>
       </c>
       <c r="K20" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="L20" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="S20" t="s">
         <v>97</v>
@@ -1417,28 +1438,28 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H21" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="J21" s="1">
-        <v>44573.75</v>
+        <v>44574.75</v>
       </c>
       <c r="K21" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="L21" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="S21" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.2">
@@ -1464,13 +1485,13 @@
         <v>44573.75</v>
       </c>
       <c r="K22" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="L22" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="S22" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.2">
@@ -1502,7 +1523,7 @@
         <v>86</v>
       </c>
       <c r="S23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.2">
@@ -1534,7 +1555,7 @@
         <v>86</v>
       </c>
       <c r="S24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.2">
@@ -1566,7 +1587,7 @@
         <v>86</v>
       </c>
       <c r="S25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.2">
@@ -1598,7 +1619,7 @@
         <v>86</v>
       </c>
       <c r="S26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.2">
@@ -1630,7 +1651,7 @@
         <v>86</v>
       </c>
       <c r="S27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.2">
@@ -1662,7 +1683,7 @@
         <v>86</v>
       </c>
       <c r="S28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.2">
@@ -1694,7 +1715,7 @@
         <v>86</v>
       </c>
       <c r="S29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.2">
@@ -1726,7 +1747,7 @@
         <v>86</v>
       </c>
       <c r="S30" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.2">
@@ -1752,19 +1773,13 @@
         <v>44573.75</v>
       </c>
       <c r="K31" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="L31" t="s">
-        <v>25</v>
-      </c>
-      <c r="O31" t="s">
-        <v>2</v>
-      </c>
-      <c r="P31" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="S31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.2">
@@ -1802,7 +1817,7 @@
         <v>36</v>
       </c>
       <c r="S32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="3:19" x14ac:dyDescent="0.2">
@@ -1840,7 +1855,7 @@
         <v>36</v>
       </c>
       <c r="S33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.2">
@@ -1878,27 +1893,45 @@
         <v>36</v>
       </c>
       <c r="S34" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="E35" s="1">
         <v>44575.086921296293</v>
       </c>
       <c r="F35" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="G35" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" s="1">
+        <v>44573.75</v>
+      </c>
+      <c r="K35" t="s">
+        <v>81</v>
       </c>
       <c r="L35" t="s">
+        <v>25</v>
+      </c>
+      <c r="O35" t="s">
         <v>2</v>
       </c>
-      <c r="M35" t="s">
+      <c r="P35" t="s">
         <v>36</v>
       </c>
       <c r="S35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="3:19" x14ac:dyDescent="0.2">
@@ -1911,9 +1944,6 @@
       <c r="F36" t="s">
         <v>29</v>
       </c>
-      <c r="G36" t="s">
-        <v>60</v>
-      </c>
       <c r="L36" t="s">
         <v>2</v>
       </c>
@@ -1921,7 +1951,7 @@
         <v>36</v>
       </c>
       <c r="S36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="3:19" x14ac:dyDescent="0.2">
@@ -1932,7 +1962,10 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F37" t="s">
-        <v>74</v>
+        <v>29</v>
+      </c>
+      <c r="G37" t="s">
+        <v>60</v>
       </c>
       <c r="L37" t="s">
         <v>2</v>
@@ -1941,12 +1974,12 @@
         <v>36</v>
       </c>
       <c r="S37" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E38" s="1">
         <v>44575.086921296293</v>
@@ -1954,34 +1987,34 @@
       <c r="F38" t="s">
         <v>74</v>
       </c>
-      <c r="K38" t="s">
-        <v>18</v>
-      </c>
       <c r="L38" t="s">
-        <v>73</v>
+        <v>2</v>
+      </c>
+      <c r="M38" t="s">
+        <v>36</v>
       </c>
       <c r="S38" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="E39" s="1">
         <v>44575.086921296293</v>
       </c>
       <c r="F39" t="s">
-        <v>29</v>
-      </c>
-      <c r="G39" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="K39" t="s">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="L39" t="s">
+        <v>73</v>
       </c>
       <c r="S39" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="3:19" x14ac:dyDescent="0.2">
@@ -1995,13 +2028,13 @@
         <v>29</v>
       </c>
       <c r="G40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K40" t="s">
         <v>3</v>
       </c>
       <c r="S40" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="3:19" x14ac:dyDescent="0.2">
@@ -2015,13 +2048,13 @@
         <v>29</v>
       </c>
       <c r="G41" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K41" t="s">
         <v>3</v>
       </c>
       <c r="S41" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="3:19" x14ac:dyDescent="0.2">
@@ -2035,16 +2068,13 @@
         <v>29</v>
       </c>
       <c r="G42" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="K42" t="s">
         <v>3</v>
       </c>
-      <c r="P42" t="s">
-        <v>1</v>
-      </c>
       <c r="S42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="3:19" x14ac:dyDescent="0.2">
@@ -2055,7 +2085,10 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F43" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="G43" t="s">
+        <v>60</v>
       </c>
       <c r="K43" t="s">
         <v>3</v>
@@ -2064,39 +2097,27 @@
         <v>1</v>
       </c>
       <c r="S43" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E44" s="1">
         <v>44575.086921296293</v>
       </c>
       <c r="F44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G44" t="s">
-        <v>39</v>
-      </c>
-      <c r="H44" t="s">
-        <v>38</v>
-      </c>
-      <c r="I44" t="s">
-        <v>37</v>
-      </c>
-      <c r="J44" s="1">
-        <v>44573.75</v>
+        <v>22</v>
       </c>
       <c r="K44" t="s">
-        <v>62</v>
-      </c>
-      <c r="L44" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="P44" t="s">
+        <v>1</v>
       </c>
       <c r="S44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="3:19" x14ac:dyDescent="0.2">
@@ -2128,36 +2149,39 @@
         <v>5</v>
       </c>
       <c r="S45" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E46" s="1">
         <v>44575.086921296293</v>
       </c>
       <c r="F46" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G46" t="s">
-        <v>60</v>
+        <v>39</v>
+      </c>
+      <c r="H46" t="s">
+        <v>38</v>
       </c>
       <c r="I46" t="s">
-        <v>59</v>
+        <v>37</v>
+      </c>
+      <c r="J46" s="1">
+        <v>44573.75</v>
       </c>
       <c r="K46" t="s">
-        <v>31</v>
-      </c>
-      <c r="M46" t="s">
-        <v>34</v>
-      </c>
-      <c r="N46" t="s">
-        <v>32</v>
+        <v>62</v>
+      </c>
+      <c r="L46" t="s">
+        <v>5</v>
       </c>
       <c r="S46" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="3:19" x14ac:dyDescent="0.2">
@@ -2168,7 +2192,13 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F47" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="G47" t="s">
+        <v>60</v>
+      </c>
+      <c r="I47" t="s">
+        <v>59</v>
       </c>
       <c r="K47" t="s">
         <v>31</v>
@@ -2180,7 +2210,7 @@
         <v>32</v>
       </c>
       <c r="S47" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="3:19" x14ac:dyDescent="0.2">
@@ -2191,68 +2221,56 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F48" t="s">
+        <v>40</v>
+      </c>
+      <c r="K48" t="s">
+        <v>31</v>
+      </c>
+      <c r="M48" t="s">
+        <v>34</v>
+      </c>
+      <c r="N48" t="s">
+        <v>32</v>
+      </c>
+      <c r="S48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F49" t="s">
         <v>29</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>55</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K49" t="s">
         <v>54</v>
       </c>
-      <c r="L48" t="s">
+      <c r="L49" t="s">
         <v>31</v>
       </c>
-      <c r="N48" t="s">
+      <c r="N49" t="s">
         <v>26</v>
       </c>
-      <c r="O48" t="s">
+      <c r="O49" t="s">
         <v>25</v>
       </c>
-      <c r="S48" t="s">
+      <c r="S49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
-        <v>41</v>
-      </c>
-      <c r="E49" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F49" t="s">
-        <v>40</v>
-      </c>
-      <c r="G49" t="s">
-        <v>39</v>
-      </c>
-      <c r="H49" t="s">
-        <v>38</v>
-      </c>
-      <c r="I49" t="s">
-        <v>37</v>
-      </c>
-      <c r="J49" s="1">
-        <v>44573.75</v>
-      </c>
-      <c r="K49" t="s">
-        <v>44</v>
-      </c>
-      <c r="L49" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>3</v>
-      </c>
-      <c r="S49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>41</v>
       </c>
       <c r="E50" s="1">
-        <v>44532.586909722224</v>
+        <v>44575.086921296293</v>
       </c>
       <c r="F50" t="s">
         <v>40</v>
@@ -2264,27 +2282,30 @@
         <v>38</v>
       </c>
       <c r="I50" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="J50" s="1">
-        <v>44531.75</v>
+        <v>44573.75</v>
       </c>
       <c r="K50" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="L50" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>3</v>
       </c>
       <c r="S50" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
         <v>41</v>
       </c>
       <c r="E51" s="1">
-        <v>44575.086921296293</v>
+        <v>44532.586909722224</v>
       </c>
       <c r="F51" t="s">
         <v>40</v>
@@ -2296,10 +2317,10 @@
         <v>38</v>
       </c>
       <c r="I51" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="J51" s="1">
-        <v>44573.75</v>
+        <v>44531.75</v>
       </c>
       <c r="K51" t="s">
         <v>2</v>
@@ -2308,15 +2329,15 @@
         <v>36</v>
       </c>
       <c r="S51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
         <v>41</v>
       </c>
       <c r="E52" s="1">
-        <v>44574.086898148147</v>
+        <v>44575.086921296293</v>
       </c>
       <c r="F52" t="s">
         <v>40</v>
@@ -2328,22 +2349,22 @@
         <v>38</v>
       </c>
       <c r="I52" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="J52" s="1">
-        <v>44570.75</v>
+        <v>44573.75</v>
       </c>
       <c r="K52" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="L52" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="S52" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
         <v>41</v>
       </c>
@@ -2351,16 +2372,16 @@
         <v>44574.086898148147</v>
       </c>
       <c r="F53" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G53" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H53" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I53" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J53" s="1">
         <v>44570.75</v>
@@ -2371,14 +2392,11 @@
       <c r="L53" t="s">
         <v>43</v>
       </c>
-      <c r="Q53" t="s">
-        <v>26</v>
-      </c>
       <c r="S53" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
         <v>41</v>
       </c>
@@ -2389,7 +2407,16 @@
         <v>29</v>
       </c>
       <c r="G54" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="H54" t="s">
+        <v>47</v>
+      </c>
+      <c r="I54" t="s">
+        <v>46</v>
+      </c>
+      <c r="J54" s="1">
+        <v>44570.75</v>
       </c>
       <c r="K54" t="s">
         <v>44</v>
@@ -2404,65 +2431,65 @@
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
         <v>41</v>
       </c>
       <c r="E55" s="1">
-        <v>44575.086921296293</v>
+        <v>44574.086898148147</v>
       </c>
       <c r="F55" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" t="s">
+        <v>45</v>
+      </c>
+      <c r="K55" t="s">
+        <v>44</v>
+      </c>
+      <c r="L55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>26</v>
+      </c>
+      <c r="S55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F56" t="s">
         <v>40</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>39</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H56" t="s">
         <v>38</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I56" t="s">
         <v>37</v>
       </c>
-      <c r="J55" s="1">
+      <c r="J56" s="1">
         <v>44573.75</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K56" t="s">
         <v>2</v>
       </c>
-      <c r="L55" t="s">
+      <c r="L56" t="s">
         <v>36</v>
       </c>
-      <c r="S55" t="s">
+      <c r="S56" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C56" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F56" t="s">
-        <v>27</v>
-      </c>
-      <c r="K56" t="s">
-        <v>34</v>
-      </c>
-      <c r="L56" t="s">
-        <v>33</v>
-      </c>
-      <c r="O56" t="s">
-        <v>32</v>
-      </c>
-      <c r="P56" t="s">
-        <v>31</v>
-      </c>
-      <c r="S56" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
         <v>20</v>
       </c>
@@ -2470,19 +2497,25 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F57" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K57" t="s">
-        <v>26</v>
-      </c>
-      <c r="M57" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="L57" t="s">
+        <v>33</v>
+      </c>
+      <c r="O57" t="s">
+        <v>32</v>
+      </c>
+      <c r="P57" t="s">
+        <v>31</v>
       </c>
       <c r="S57" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
         <v>20</v>
       </c>
@@ -2490,7 +2523,7 @@
         <v>44575.086921296293</v>
       </c>
       <c r="F58" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K58" t="s">
         <v>26</v>
@@ -2499,100 +2532,67 @@
         <v>25</v>
       </c>
       <c r="S58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F59" t="s">
+        <v>27</v>
+      </c>
+      <c r="K59" t="s">
+        <v>26</v>
+      </c>
+      <c r="M59" t="s">
+        <v>25</v>
+      </c>
+      <c r="S59" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C59" t="s">
+    <row r="60" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
         <v>23</v>
       </c>
-      <c r="E59" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E60" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F60" t="s">
         <v>22</v>
-      </c>
-      <c r="K59" t="s">
-        <v>3</v>
-      </c>
-      <c r="P59" t="s">
-        <v>1</v>
-      </c>
-      <c r="S59" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
-        <v>20</v>
-      </c>
-      <c r="E60" s="1">
-        <v>44575.086921296293</v>
-      </c>
-      <c r="F60" t="s">
-        <v>19</v>
       </c>
       <c r="K60" t="s">
         <v>3</v>
       </c>
-      <c r="M60" t="s">
+      <c r="P60" t="s">
+        <v>1</v>
+      </c>
+      <c r="S60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" s="1">
+        <v>44575.086921296293</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="K61" t="s">
+        <v>3</v>
+      </c>
+      <c r="M61" t="s">
         <v>18</v>
       </c>
-      <c r="S60" t="s">
+      <c r="S61" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" t="s">
-        <v>11</v>
-      </c>
-      <c r="G61" t="s">
-        <v>10</v>
-      </c>
-      <c r="H61" t="s">
-        <v>9</v>
-      </c>
-      <c r="I61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J61" t="s">
-        <v>7</v>
-      </c>
-      <c r="K61" t="s">
-        <v>6</v>
-      </c>
-      <c r="L61" t="s">
-        <v>5</v>
-      </c>
-      <c r="M61" t="s">
-        <v>4</v>
-      </c>
-      <c r="N61" t="s">
-        <v>3</v>
-      </c>
-      <c r="P61" t="s">
-        <v>2</v>
-      </c>
-      <c r="R61" t="s">
-        <v>1</v>
-      </c>
-      <c r="S61" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>